<commit_message>
add logic to automate the date
</commit_message>
<xml_diff>
--- a/test-output/excel-report.xlsx
+++ b/test-output/excel-report.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -42,19 +42,19 @@
     <t>Start Time</t>
   </si>
   <si>
-    <t>2021-06-03T01:21:32 IST</t>
+    <t>2021-06-03T01:27:23 IST</t>
   </si>
   <si>
     <t>End Time</t>
   </si>
   <si>
-    <t>2021-06-03T01:22:39 IST</t>
+    <t>2021-06-03T01:28:21 IST</t>
   </si>
   <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>67363 ms</t>
+    <t>57702 ms</t>
   </si>
   <si>
     <t>TestCase Name</t>
@@ -75,25 +75,22 @@
     <t/>
   </si>
   <si>
-    <t>2021-06-03T01:21:56 IST</t>
-  </si>
-  <si>
-    <t>2021-06-03T01:22:03 IST</t>
-  </si>
-  <si>
-    <t>7890 ms</t>
+    <t>2021-06-03T01:27:42 IST</t>
+  </si>
+  <si>
+    <t>2021-06-03T01:27:49 IST</t>
+  </si>
+  <si>
+    <t>7848 ms</t>
   </si>
   <si>
     <t>com.bridgelabz.test.LoginModuleTest.logoutPageTest</t>
   </si>
   <si>
-    <t>2021-06-03T01:22:04 IST</t>
-  </si>
-  <si>
-    <t>2021-06-03T01:22:24 IST</t>
-  </si>
-  <si>
-    <t>20054 ms</t>
+    <t>2021-06-03T01:28:07 IST</t>
+  </si>
+  <si>
+    <t>17768 ms</t>
   </si>
 </sst>
 </file>
@@ -450,13 +447,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="F3" s="36" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>